<commit_message>
weiter Aufgabe 2-8 PDF und excel
</commit_message>
<xml_diff>
--- a/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
+++ b/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgb1" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>AccessCount</t>
   </si>
@@ -54,21 +54,6 @@
     <t>Average number of elements</t>
   </si>
   <si>
-    <t>MatrixList</t>
-  </si>
-  <si>
-    <t>MatrixArrayList</t>
-  </si>
-  <si>
-    <t>n=1</t>
-  </si>
-  <si>
-    <t>Overhead:</t>
-  </si>
-  <si>
-    <t>t=500 für große Genauigkeit</t>
-  </si>
-  <si>
     <t>Aufgabe 7</t>
   </si>
   <si>
@@ -145,6 +130,27 @@
   </si>
   <si>
     <t>Variance</t>
+  </si>
+  <si>
+    <t>Average NoOfElements MatrixList</t>
+  </si>
+  <si>
+    <t>Average NoOfElements MatrixArrayList</t>
+  </si>
+  <si>
+    <t>Average NoOfElements MatrixArray</t>
+  </si>
+  <si>
+    <t>Versuch 2:</t>
+  </si>
+  <si>
+    <t>Versuch 1:</t>
+  </si>
+  <si>
+    <t>p=0.01</t>
+  </si>
+  <si>
+    <t>Operation ist die Addition</t>
   </si>
 </sst>
 </file>
@@ -354,9 +360,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -438,25 +442,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50237440"/>
-        <c:axId val="50238976"/>
+        <c:axId val="73700096"/>
+        <c:axId val="73701632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50237440"/>
+        <c:axId val="73700096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50238976"/>
+        <c:crossAx val="73701632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50238976"/>
+        <c:axId val="73701632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -464,20 +468,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50237440"/>
+        <c:crossAx val="73700096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -487,17 +490,16 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10812550723840972"/>
+          <c:x val="0.10812550723840979"/>
           <c:y val="0.14061001832402045"/>
-          <c:w val="0.64893491042327311"/>
-          <c:h val="0.77567520489538722"/>
+          <c:w val="0.64893491042327356"/>
+          <c:h val="0.77567520489538766"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -548,26 +550,54 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MatrixArray</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Aufgb2!$C$20:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="89854720"/>
-        <c:axId val="89856256"/>
+        <c:axId val="79211904"/>
+        <c:axId val="79221888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89854720"/>
+        <c:axId val="79211904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89856256"/>
+        <c:crossAx val="79221888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89856256"/>
+        <c:axId val="79221888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,19 +605,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89854720"/>
+        <c:crossAx val="79211904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -612,7 +643,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Aufgb2!$B$40:$B$42</c:f>
+              <c:f>Aufgb2!$B$31:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -630,7 +661,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$40:$C$42</c:f>
+              <c:f>Aufgb2!$C$31:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -658,7 +689,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$46:$C$48</c:f>
+              <c:f>Aufgb2!$C$37:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -686,7 +717,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$52:$C$54</c:f>
+              <c:f>Aufgb2!$C$43:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -714,7 +745,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$58:$C$60</c:f>
+              <c:f>Aufgb2!$C$49:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -732,25 +763,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="89903872"/>
-        <c:axId val="89905408"/>
+        <c:axId val="79252096"/>
+        <c:axId val="79262080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89903872"/>
+        <c:axId val="79252096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89905408"/>
+        <c:crossAx val="79262080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89905408"/>
+        <c:axId val="79262080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -759,19 +790,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89903872"/>
+        <c:crossAx val="79252096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1373,25 +1405,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91773568"/>
-        <c:axId val="91787648"/>
+        <c:axId val="81208064"/>
+        <c:axId val="81209600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91773568"/>
+        <c:axId val="81208064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91787648"/>
+        <c:crossAx val="81209600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91787648"/>
+        <c:axId val="81209600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,20 +1431,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91773568"/>
+        <c:crossAx val="81208064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1457,16 +1488,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1489,13 +1520,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1840,7 +1871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1853,7 +1884,7 @@
   <sheetData>
     <row r="5" spans="1:4" ht="15.75" thickBot="1">
       <c r="A5" s="12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
@@ -1909,7 +1940,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
       <c r="A13" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
@@ -1952,7 +1983,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1">
       <c r="A19" s="12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1967,10 +1998,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1981,7 +2012,7 @@
         <v>814</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2007,10 +2038,10 @@
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2024,7 +2055,7 @@
         <v>2985</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F24" s="22">
         <v>2924</v>
@@ -2086,10 +2117,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D60"/>
+  <dimension ref="A3:D54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="A3:C18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2102,7 +2133,7 @@
   <sheetData>
     <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2126,7 +2157,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2166,7 +2197,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2193,287 +2224,256 @@
         <v>99693.4</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="2" t="s">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B22" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D30" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="15.75" thickBot="1"/>
-    <row r="25" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B25" s="9" t="s">
+    <row r="31" spans="1:4">
+      <c r="B31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C31" s="13">
+        <v>142015.66666700001</v>
+      </c>
+      <c r="D31" s="14">
+        <v>474503863.66666698</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="B32" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C32" s="13">
+        <v>622421</v>
+      </c>
+      <c r="D32" s="14">
+        <v>2912721758.1428499</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B33" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C33" s="15">
+        <v>1249198.733333</v>
+      </c>
+      <c r="D33" s="16">
+        <v>2165148774.0666599</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="36" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B36" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="3">
+      <c r="C36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="3">
         <v>0.01</v>
       </c>
-      <c r="C26" s="5">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="3">
+      <c r="C37" s="13">
+        <v>8520940</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1708213909200</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="3">
         <v>0.05</v>
       </c>
-      <c r="C27" s="5">
-        <v>5.6000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B28" s="6">
+      <c r="C38" s="13">
+        <v>37345260</v>
+      </c>
+      <c r="D38" s="14">
+        <v>10485798329314.199</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B39" s="6">
         <v>0.1</v>
       </c>
-      <c r="C28" s="8">
-        <v>0.11799999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B31" s="9" t="s">
+      <c r="C39" s="15">
+        <v>74951924</v>
+      </c>
+      <c r="D39" s="16">
+        <v>7794535586640</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="42" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B42" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="3">
+      <c r="C42" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="3">
         <v>0.01</v>
       </c>
-      <c r="C32" s="5">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="B33" s="3">
+      <c r="C43" s="13">
+        <v>2365.9333329999999</v>
+      </c>
+      <c r="D43" s="14">
+        <v>131114.06666700001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="3">
         <v>0.05</v>
       </c>
-      <c r="C33" s="5">
-        <v>5.6000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B34" s="6">
+      <c r="C44" s="13">
+        <v>10383</v>
+      </c>
+      <c r="D44" s="14">
+        <v>822370</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B45" s="6">
         <v>0.1</v>
       </c>
-      <c r="C34" s="8">
-        <v>0.11799999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C45" s="15">
+        <v>20835.866666999998</v>
+      </c>
+      <c r="D45" s="16">
+        <v>7794535586640</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="48" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B48" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="B40" s="3">
+      <c r="D48" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="3">
         <v>0.01</v>
       </c>
-      <c r="C40" s="13">
-        <v>142015.66666700001</v>
-      </c>
-      <c r="D40" s="14">
-        <v>474503863.66666698</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="B41" s="3">
+      <c r="C49" s="13">
+        <v>141956</v>
+      </c>
+      <c r="D49" s="14">
+        <v>472010640</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="3">
         <v>0.05</v>
       </c>
-      <c r="C41" s="13">
-        <v>622421</v>
-      </c>
-      <c r="D41" s="14">
-        <v>2912721758.1428499</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B42" s="6">
+      <c r="C50" s="13">
+        <v>622980</v>
+      </c>
+      <c r="D50" s="14">
+        <v>2960532000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B51" s="6">
         <v>0.1</v>
       </c>
-      <c r="C42" s="15">
-        <v>1249198.733333</v>
-      </c>
-      <c r="D42" s="16">
-        <v>2165148774.0666599</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B45" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="B46" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C46" s="13">
-        <v>8520940</v>
-      </c>
-      <c r="D46" s="14">
-        <v>1708213909200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="B47" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="C47" s="13">
-        <v>37345260</v>
-      </c>
-      <c r="D47" s="14">
-        <v>10485798329314.199</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B48" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C48" s="15">
-        <v>74951924</v>
-      </c>
-      <c r="D48" s="16">
-        <v>7794535586640</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="51" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B51" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C52" s="13">
-        <v>2365.9333329999999</v>
-      </c>
-      <c r="D52" s="14">
-        <v>131114.06666700001</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="C53" s="13">
-        <v>10383</v>
-      </c>
-      <c r="D53" s="14">
-        <v>822370</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B54" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C54" s="15">
-        <v>20835.866666999998</v>
-      </c>
-      <c r="D54" s="16">
-        <v>7794535586640</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="57" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B57" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4">
-      <c r="B58" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C58" s="13">
-        <v>141956</v>
-      </c>
-      <c r="D58" s="14">
-        <v>472010640</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4">
-      <c r="B59" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="C59" s="13">
-        <v>622980</v>
-      </c>
-      <c r="D59" s="14">
-        <v>2960532000</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B60" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C60" s="15">
+      <c r="C51" s="15">
         <v>1250152</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D51" s="16">
         <v>2135479817.1428499</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2493,20 +2493,20 @@
   <sheetData>
     <row r="3" spans="1:4">
       <c r="A3" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1">
@@ -2514,13 +2514,13 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1">
       <c r="B7" s="19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">

</xml_diff>

<commit_message>
aufgabe 1 und 2 finished
</commit_message>
<xml_diff>
--- a/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
+++ b/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>AccessCount</t>
   </si>
@@ -69,12 +69,6 @@
     <t>ListenAdd Variance</t>
   </si>
   <si>
-    <t>n=60</t>
-  </si>
-  <si>
-    <t>t=15</t>
-  </si>
-  <si>
     <t>ListenMult Average</t>
   </si>
   <si>
@@ -141,16 +135,16 @@
     <t>Average NoOfElements MatrixArray</t>
   </si>
   <si>
-    <t>Versuch 2:</t>
-  </si>
-  <si>
-    <t>Versuch 1:</t>
-  </si>
-  <si>
-    <t>p=0.01</t>
-  </si>
-  <si>
-    <t>Operation ist die Addition</t>
+    <t>Versuch 1: Anzahl der Dereferenzierungen</t>
+  </si>
+  <si>
+    <t>n=</t>
+  </si>
+  <si>
+    <t>t=</t>
+  </si>
+  <si>
+    <t>Overhead - AccessCount/n²</t>
   </si>
 </sst>
 </file>
@@ -283,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,13 +316,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -346,6 +334,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,25 +437,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73700096"/>
-        <c:axId val="73701632"/>
+        <c:axId val="83399424"/>
+        <c:axId val="83400960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73700096"/>
+        <c:axId val="83399424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73701632"/>
+        <c:crossAx val="83400960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73701632"/>
+        <c:axId val="83400960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +463,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73700096"/>
+        <c:crossAx val="83399424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -480,7 +475,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -496,10 +491,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10812550723840979"/>
+          <c:x val="0.10812550723840986"/>
           <c:y val="0.14061001832402045"/>
-          <c:w val="0.64893491042327356"/>
-          <c:h val="0.77567520489538766"/>
+          <c:w val="0.64893491042327411"/>
+          <c:h val="0.7756752048953881"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -579,25 +574,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="79211904"/>
-        <c:axId val="79221888"/>
+        <c:axId val="83733888"/>
+        <c:axId val="83752064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79211904"/>
+        <c:axId val="83733888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79221888"/>
+        <c:crossAx val="83752064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79221888"/>
+        <c:axId val="83752064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +600,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79211904"/>
+        <c:crossAx val="83733888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -618,7 +613,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -763,25 +758,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="79252096"/>
-        <c:axId val="79262080"/>
+        <c:axId val="88304256"/>
+        <c:axId val="88314240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79252096"/>
+        <c:axId val="88304256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79262080"/>
+        <c:crossAx val="88314240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79262080"/>
+        <c:axId val="88314240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -790,7 +785,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79252096"/>
+        <c:crossAx val="88304256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -803,13 +798,180 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ListAdd Overhead</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Aufgb2!$E$31:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.448796296388892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>172.89472222222221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>346.99964814805554</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ListMult Overhead</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Aufgb2!$E$37:$E$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2366.9277777777775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10373.683333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20819.978888888891</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ArrayListAdd Overhead</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Aufgb2!$E$43:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.65720370361111113</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8841666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7877407408333328</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>ArrayListMult Overhead</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Aufgb2!$E$49:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.432222222222222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>347.26444444444439</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="88340352"/>
+        <c:axId val="88341888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88340352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88341888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88341888"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88340352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
@@ -1405,25 +1567,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81208064"/>
-        <c:axId val="81209600"/>
+        <c:axId val="90374144"/>
+        <c:axId val="90375680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81208064"/>
+        <c:axId val="90374144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81209600"/>
+        <c:crossAx val="90375680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81209600"/>
+        <c:axId val="90375680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1593,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81208064"/>
+        <c:crossAx val="90374144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1443,7 +1605,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1489,15 +1651,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>409574</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:colOff>1720662</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68354</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>310402</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>58830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1518,16 +1680,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>18331</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>72965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>889620</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>72964</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1541,6 +1703,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1075767</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131703</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>44822</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1998,10 +2190,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2011,8 +2203,8 @@
       <c r="C21" s="4">
         <v>814</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>32</v>
+      <c r="D21" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2022,7 +2214,7 @@
       <c r="C22" s="4">
         <v>820</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="18">
         <v>2683.2999999999302</v>
       </c>
     </row>
@@ -2033,15 +2225,15 @@
       <c r="C23" s="4">
         <v>828</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="18">
         <v>3189</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>37</v>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2051,16 +2243,16 @@
       <c r="C24" s="4">
         <v>797</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="18">
         <v>2985</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="22">
+      <c r="E24" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="20">
         <v>2924</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="20">
         <v>47492</v>
       </c>
     </row>
@@ -2071,7 +2263,7 @@
       <c r="C25" s="4">
         <v>789</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="18">
         <v>3878</v>
       </c>
     </row>
@@ -2082,7 +2274,7 @@
       <c r="C26" s="4">
         <v>792</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="18">
         <v>4031</v>
       </c>
     </row>
@@ -2093,7 +2285,7 @@
       <c r="C27" s="4">
         <v>794</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="18">
         <v>3666</v>
       </c>
     </row>
@@ -2104,7 +2296,7 @@
       <c r="C28" s="7">
         <v>795</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="19">
         <v>3751</v>
       </c>
     </row>
@@ -2117,18 +2309,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D54"/>
+  <dimension ref="A3:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="2" max="5" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -2157,7 +2347,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2197,7 +2387,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2224,16 +2414,16 @@
         <v>99693.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1">
       <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="B20" s="3">
         <v>0.01</v>
       </c>
@@ -2241,7 +2431,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="B21" s="3">
         <v>0.05</v>
       </c>
@@ -2249,7 +2439,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1">
       <c r="B22" s="6">
         <v>0.1</v>
       </c>
@@ -2257,217 +2447,306 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="B27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1">
+        <v>39</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="D28" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1">
       <c r="B30" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="B31" s="3">
         <v>0.01</v>
       </c>
       <c r="C31" s="13">
         <v>142015.66666700001</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="13">
         <v>474503863.66666698</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="5">
+        <f>C31/$E$27/$E$27</f>
+        <v>39.448796296388892</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="B32" s="3">
         <v>0.05</v>
       </c>
       <c r="C32" s="13">
         <v>622421</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="13">
         <v>2912721758.1428499</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1">
+      <c r="E32" s="5">
+        <f>C32/$E$27/$E$27</f>
+        <v>172.89472222222221</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" thickBot="1">
       <c r="B33" s="6">
         <v>0.1</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>1249198.733333</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="14">
         <v>2165148774.0666599</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="36" spans="2:4" ht="15.75" thickBot="1">
+      <c r="E33" s="8">
+        <f>C33/$E$27/$E$27</f>
+        <v>346.99964814805554</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" thickBot="1">
       <c r="B36" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
+        <v>17</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
       <c r="B37" s="3">
         <v>0.01</v>
       </c>
       <c r="C37" s="13">
         <v>8520940</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="13">
         <v>1708213909200</v>
       </c>
-    </row>
-    <row r="38" spans="2:4">
+      <c r="E37" s="5">
+        <f>C37/$E$27/$E$27</f>
+        <v>2366.9277777777775</v>
+      </c>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="2:9">
       <c r="B38" s="3">
         <v>0.05</v>
       </c>
       <c r="C38" s="13">
         <v>37345260</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="13">
         <v>10485798329314.199</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" ht="15.75" thickBot="1">
+      <c r="E38" s="5">
+        <f>C38/$E$27/$E$27</f>
+        <v>10373.683333333332</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" thickBot="1">
       <c r="B39" s="6">
         <v>0.1</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="14">
         <v>74951924</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="14">
         <v>7794535586640</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="42" spans="2:4" ht="15.75" thickBot="1">
+      <c r="E39" s="8">
+        <f>C39/$E$27/$E$27</f>
+        <v>20819.978888888891</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="2:9" ht="15.75" thickBot="1">
       <c r="B42" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4">
+        <v>19</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
       <c r="B43" s="3">
         <v>0.01</v>
       </c>
       <c r="C43" s="13">
         <v>2365.9333329999999</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="13">
         <v>131114.06666700001</v>
       </c>
-    </row>
-    <row r="44" spans="2:4">
+      <c r="E43" s="5">
+        <f>C43/$E$27/$E$27</f>
+        <v>0.65720370361111113</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
       <c r="B44" s="3">
         <v>0.05</v>
       </c>
       <c r="C44" s="13">
         <v>10383</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="13">
         <v>822370</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" ht="15.75" thickBot="1">
+      <c r="E44" s="5">
+        <f>C44/$E$27/$E$27</f>
+        <v>2.8841666666666668</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="15.75" thickBot="1">
       <c r="B45" s="6">
         <v>0.1</v>
       </c>
-      <c r="C45" s="15">
+      <c r="C45" s="14">
         <v>20835.866666999998</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="14">
         <v>7794535586640</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="48" spans="2:4" ht="15.75" thickBot="1">
+      <c r="E45" s="8">
+        <f>C45/$E$27/$E$27</f>
+        <v>5.7877407408333328</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="2:9" ht="15.75" thickBot="1">
       <c r="B48" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
+        <v>21</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
       <c r="B49" s="3">
         <v>0.01</v>
       </c>
       <c r="C49" s="13">
         <v>141956</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="13">
         <v>472010640</v>
       </c>
-    </row>
-    <row r="50" spans="2:4">
+      <c r="E49" s="5">
+        <f>C49/$E$27/$E$27</f>
+        <v>39.432222222222222</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
       <c r="B50" s="3">
         <v>0.05</v>
       </c>
       <c r="C50" s="13">
         <v>622980</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50" s="13">
         <v>2960532000</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" ht="15.75" thickBot="1">
+      <c r="E50" s="5">
+        <f>C50/$E$27/$E$27</f>
+        <v>173.05</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="15.75" thickBot="1">
       <c r="B51" s="6">
         <v>0.1</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="14">
         <v>1250152</v>
       </c>
-      <c r="D51" s="16">
+      <c r="D51" s="14">
         <v>2135479817.1428499</v>
       </c>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="B54" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" t="s">
-        <v>43</v>
-      </c>
-      <c r="D54" t="s">
-        <v>44</v>
+      <c r="E51" s="8">
+        <f>C51/$E$27/$E$27</f>
+        <v>347.26444444444439</v>
       </c>
     </row>
   </sheetData>
@@ -2493,34 +2772,34 @@
   <sheetData>
     <row r="3" spans="1:4">
       <c r="A3" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2629,7 +2908,7 @@
       <c r="C17" s="4">
         <v>9</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2640,7 +2919,7 @@
       <c r="C18" s="4">
         <v>10</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2651,7 +2930,7 @@
       <c r="C19" s="4">
         <v>11</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2662,7 +2941,7 @@
       <c r="C20" s="4">
         <v>12</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2673,7 +2952,7 @@
       <c r="C21" s="4">
         <v>13</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2684,7 +2963,7 @@
       <c r="C22" s="4">
         <v>14</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2695,7 +2974,7 @@
       <c r="C23" s="4">
         <v>15</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2706,7 +2985,7 @@
       <c r="C24" s="4">
         <v>16</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2717,7 +2996,7 @@
       <c r="C25" s="4">
         <v>17</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2728,7 +3007,7 @@
       <c r="C26" s="4">
         <v>18</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2739,7 +3018,7 @@
       <c r="C27" s="4">
         <v>19</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2750,7 +3029,7 @@
       <c r="C28" s="4">
         <v>20</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2761,7 +3040,7 @@
       <c r="C29" s="4">
         <v>21</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2772,7 +3051,7 @@
       <c r="C30" s="4">
         <v>22</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2783,7 +3062,7 @@
       <c r="C31" s="4">
         <v>23</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2794,7 +3073,7 @@
       <c r="C32" s="4">
         <v>24</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2805,7 +3084,7 @@
       <c r="C33" s="4">
         <v>25</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2816,7 +3095,7 @@
       <c r="C34" s="4">
         <v>26</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2827,7 +3106,7 @@
       <c r="C35" s="4">
         <v>27</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2838,7 +3117,7 @@
       <c r="C36" s="4">
         <v>28</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2849,7 +3128,7 @@
       <c r="C37" s="4">
         <v>29</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2860,7 +3139,7 @@
       <c r="C38" s="4">
         <v>30</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2871,7 +3150,7 @@
       <c r="C39" s="4">
         <v>31</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="15">
         <v>6</v>
       </c>
     </row>
@@ -2882,7 +3161,7 @@
       <c r="C40" s="4">
         <v>32</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2893,7 +3172,7 @@
       <c r="C41" s="4">
         <v>33</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2904,7 +3183,7 @@
       <c r="C42" s="4">
         <v>34</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2915,7 +3194,7 @@
       <c r="C43" s="4">
         <v>35</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2926,7 +3205,7 @@
       <c r="C44" s="4">
         <v>36</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2937,7 +3216,7 @@
       <c r="C45" s="4">
         <v>37</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2948,7 +3227,7 @@
       <c r="C46" s="4">
         <v>38</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2959,7 +3238,7 @@
       <c r="C47" s="4">
         <v>39</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2970,7 +3249,7 @@
       <c r="C48" s="4">
         <v>40</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2981,7 +3260,7 @@
       <c r="C49" s="4">
         <v>41</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="15">
         <v>7</v>
       </c>
     </row>
@@ -2992,7 +3271,7 @@
       <c r="C50" s="4">
         <v>42</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3003,7 +3282,7 @@
       <c r="C51" s="4">
         <v>43</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3014,7 +3293,7 @@
       <c r="C52" s="4">
         <v>44</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3025,7 +3304,7 @@
       <c r="C53" s="4">
         <v>45</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D53" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3036,7 +3315,7 @@
       <c r="C54" s="4">
         <v>46</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3047,7 +3326,7 @@
       <c r="C55" s="4">
         <v>47</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3058,7 +3337,7 @@
       <c r="C56" s="4">
         <v>48</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3069,7 +3348,7 @@
       <c r="C57" s="4">
         <v>49</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D57" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3080,7 +3359,7 @@
       <c r="C58" s="4">
         <v>50</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3091,7 +3370,7 @@
       <c r="C59" s="4">
         <v>51</v>
       </c>
-      <c r="D59" s="17">
+      <c r="D59" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3102,7 +3381,7 @@
       <c r="C60" s="4">
         <v>52</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3113,7 +3392,7 @@
       <c r="C61" s="4">
         <v>53</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D61" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3124,7 +3403,7 @@
       <c r="C62" s="4">
         <v>54</v>
       </c>
-      <c r="D62" s="17">
+      <c r="D62" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3135,7 +3414,7 @@
       <c r="C63" s="4">
         <v>55</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D63" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3146,7 +3425,7 @@
       <c r="C64" s="4">
         <v>56</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3157,7 +3436,7 @@
       <c r="C65" s="4">
         <v>57</v>
       </c>
-      <c r="D65" s="17">
+      <c r="D65" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3168,7 +3447,7 @@
       <c r="C66" s="4">
         <v>58</v>
       </c>
-      <c r="D66" s="17">
+      <c r="D66" s="15">
         <v>7</v>
       </c>
     </row>
@@ -3179,7 +3458,7 @@
       <c r="C67" s="7">
         <v>59</v>
       </c>
-      <c r="D67" s="18">
+      <c r="D67" s="16">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel->printable PDFs and Abgabe.zip
</commit_message>
<xml_diff>
--- a/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
+++ b/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>AccessCount</t>
   </si>
@@ -126,15 +126,6 @@
     <t>Variance</t>
   </si>
   <si>
-    <t>Average NoOfElements MatrixList</t>
-  </si>
-  <si>
-    <t>Average NoOfElements MatrixArrayList</t>
-  </si>
-  <si>
-    <t>Average NoOfElements MatrixArray</t>
-  </si>
-  <si>
     <t>Versuch 1: Anzahl der Dereferenzierungen</t>
   </si>
   <si>
@@ -145,6 +136,18 @@
   </si>
   <si>
     <t>Overhead - AccessCount/n²</t>
+  </si>
+  <si>
+    <t>MatrixList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average NoOfElements </t>
+  </si>
+  <si>
+    <t>MatrixArrayList</t>
+  </si>
+  <si>
+    <t>MatrixArray</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -437,25 +442,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83399424"/>
-        <c:axId val="83400960"/>
+        <c:axId val="75277056"/>
+        <c:axId val="75278592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83399424"/>
+        <c:axId val="75277056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83400960"/>
+        <c:crossAx val="75278592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83400960"/>
+        <c:axId val="75278592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -463,19 +468,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83399424"/>
+        <c:crossAx val="75277056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -491,10 +497,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10812550723840986"/>
+          <c:x val="0.1081255072384099"/>
           <c:y val="0.14061001832402045"/>
-          <c:w val="0.64893491042327411"/>
-          <c:h val="0.7756752048953881"/>
+          <c:w val="0.64893491042327434"/>
+          <c:h val="0.77567520489538833"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -510,7 +516,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Aufgb2!$B$8:$B$10</c:f>
+              <c:f>Aufgb2!$B$11:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -528,7 +534,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$8:$C$10</c:f>
+              <c:f>Aufgb2!$C$11:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -556,7 +562,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$20:$C$22</c:f>
+              <c:f>Aufgb2!$C$23:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -574,25 +580,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83733888"/>
-        <c:axId val="83752064"/>
+        <c:axId val="81046912"/>
+        <c:axId val="81065088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83733888"/>
+        <c:axId val="81046912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83752064"/>
+        <c:crossAx val="81065088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83752064"/>
+        <c:axId val="81065088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +606,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83733888"/>
+        <c:crossAx val="81046912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -613,7 +619,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -638,7 +644,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Aufgb2!$B$31:$B$33</c:f>
+              <c:f>Aufgb2!$B$40:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -656,7 +662,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$31:$C$33</c:f>
+              <c:f>Aufgb2!$C$40:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -684,7 +690,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$37:$C$39</c:f>
+              <c:f>Aufgb2!$C$46:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -712,7 +718,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$43:$C$45</c:f>
+              <c:f>Aufgb2!$C$52:$C$54</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -740,7 +746,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$C$49:$C$51</c:f>
+              <c:f>Aufgb2!$C$58:$C$60</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -758,25 +764,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88304256"/>
-        <c:axId val="88314240"/>
+        <c:axId val="82401920"/>
+        <c:axId val="82416000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88304256"/>
+        <c:axId val="82401920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88314240"/>
+        <c:crossAx val="82416000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88314240"/>
+        <c:axId val="82416000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -785,20 +791,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88304256"/>
+        <c:crossAx val="82401920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -823,7 +829,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$E$31:$E$33</c:f>
+              <c:f>Aufgb2!$E$40:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -851,7 +857,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$E$37:$E$39</c:f>
+              <c:f>Aufgb2!$E$46:$E$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -879,7 +885,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$E$43:$E$45</c:f>
+              <c:f>Aufgb2!$E$52:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -907,7 +913,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Aufgb2!$E$49:$E$51</c:f>
+              <c:f>Aufgb2!$E$58:$E$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -925,25 +931,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88340352"/>
-        <c:axId val="88341888"/>
+        <c:axId val="82446208"/>
+        <c:axId val="82447744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88340352"/>
+        <c:axId val="82446208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88341888"/>
+        <c:crossAx val="82447744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88341888"/>
+        <c:axId val="82447744"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -952,20 +958,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88340352"/>
+        <c:crossAx val="82446208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1567,25 +1573,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="90374144"/>
-        <c:axId val="90375680"/>
+        <c:axId val="82509824"/>
+        <c:axId val="82511360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90374144"/>
+        <c:axId val="82509824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90375680"/>
+        <c:crossAx val="82511360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90375680"/>
+        <c:axId val="82511360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1593,19 +1599,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90374144"/>
+        <c:crossAx val="82509824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1616,15 +1623,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>362630</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121784</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>343580</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>7484</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1651,15 +1658,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1720662</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:colOff>387163</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>68354</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>310402</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>357189</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>58830</xdr:rowOff>
+      <xdr:rowOff>32651</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1680,16 +1687,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>18331</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>72965</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>452438</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>144403</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>889620</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>72964</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1143001</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1710,16 +1717,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1075767</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1595437</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>116263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>131703</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>44822</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>346015</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>142877</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2063,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2302,456 +2309,465 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:I51"/>
+  <dimension ref="A6:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="5" width="32.28515625" customWidth="1"/>
+    <col min="2" max="5" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3">
-      <c r="A3" s="12" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="2" t="s">
+    <row r="7" spans="1:3">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="1" t="s">
+    <row r="8" spans="1:3">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B7" s="9" t="s">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C10" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="5">
+        <v>9946</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C12" s="5">
+        <v>50088.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B13" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="8">
+        <v>99693.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C17" s="5">
+        <v>9946</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="5">
+        <v>50088.2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B19" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>99693.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" thickBot="1">
+      <c r="C21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B25" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="B36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="3">
+      <c r="D36" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="D37" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="21">
+        <v>15</v>
+      </c>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1">
+      <c r="B39" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="B40" s="3">
         <v>0.01</v>
       </c>
-      <c r="C8" s="5">
-        <v>9946</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="3">
+      <c r="C40" s="13">
+        <v>142015.66666700001</v>
+      </c>
+      <c r="D40" s="13">
+        <v>474503863.66666698</v>
+      </c>
+      <c r="E40" s="5">
+        <f>C40/$E$36/$E$36</f>
+        <v>39.448796296388892</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="B41" s="3">
         <v>0.05</v>
       </c>
-      <c r="C9" s="5">
-        <v>50088.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B10" s="6">
+      <c r="C41" s="13">
+        <v>622421</v>
+      </c>
+      <c r="D41" s="13">
+        <v>2912721758.1428499</v>
+      </c>
+      <c r="E41" s="5">
+        <f>C41/$E$36/$E$36</f>
+        <v>172.89472222222221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1">
+      <c r="B42" s="6">
         <v>0.1</v>
       </c>
-      <c r="C10" s="8">
-        <v>99693.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B13" s="9" t="s">
+      <c r="C42" s="14">
+        <v>1249198.733333</v>
+      </c>
+      <c r="D42" s="14">
+        <v>2165148774.0666599</v>
+      </c>
+      <c r="E42" s="8">
+        <f>C42/$E$36/$E$36</f>
+        <v>346.99964814805554</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" thickBot="1">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1">
+      <c r="B45" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="3">
+      <c r="C45" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="B46" s="3">
         <v>0.01</v>
       </c>
-      <c r="C14" s="5">
-        <v>9946</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="3">
+      <c r="C46" s="13">
+        <v>8520940</v>
+      </c>
+      <c r="D46" s="13">
+        <v>1708213909200</v>
+      </c>
+      <c r="E46" s="5">
+        <f>C46/$E$36/$E$36</f>
+        <v>2366.9277777777775</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="B47" s="3">
         <v>0.05</v>
       </c>
-      <c r="C15" s="5">
-        <v>50088.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B16" s="6">
+      <c r="C47" s="13">
+        <v>37345260</v>
+      </c>
+      <c r="D47" s="13">
+        <v>10485798329314.199</v>
+      </c>
+      <c r="E47" s="5">
+        <f>C47/$E$36/$E$36</f>
+        <v>10373.683333333332</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" thickBot="1">
+      <c r="B48" s="6">
         <v>0.1</v>
       </c>
-      <c r="C16" s="8">
-        <v>99693.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1"/>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B19" s="9" t="s">
+      <c r="C48" s="14">
+        <v>74951924</v>
+      </c>
+      <c r="D48" s="14">
+        <v>7794535586640</v>
+      </c>
+      <c r="E48" s="8">
+        <f>C48/$E$36/$E$36</f>
+        <v>20819.978888888891</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B51" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" s="3">
+      <c r="C51" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" s="3">
         <v>0.01</v>
       </c>
-      <c r="C20" s="5">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" s="3">
+      <c r="C52" s="13">
+        <v>2365.9333329999999</v>
+      </c>
+      <c r="D52" s="13">
+        <v>131114.06666700001</v>
+      </c>
+      <c r="E52" s="5">
+        <f>C52/$E$36/$E$36</f>
+        <v>0.65720370361111113</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="B53" s="3">
         <v>0.05</v>
       </c>
-      <c r="C21" s="5">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B22" s="6">
+      <c r="C53" s="13">
+        <v>10383</v>
+      </c>
+      <c r="D53" s="13">
+        <v>822370</v>
+      </c>
+      <c r="E53" s="5">
+        <f>C53/$E$36/$E$36</f>
+        <v>2.8841666666666668</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B54" s="6">
         <v>0.1</v>
       </c>
-      <c r="C22" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
+      <c r="C54" s="14">
+        <v>20835.866666999998</v>
+      </c>
+      <c r="D54" s="14">
+        <v>7794535586640</v>
+      </c>
+      <c r="E54" s="8">
+        <f>C54/$E$36/$E$36</f>
+        <v>5.7877407408333328</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B57" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="21">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="D28" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="21">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1"/>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" s="3">
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="3">
         <v>0.01</v>
       </c>
-      <c r="C31" s="13">
-        <v>142015.66666700001</v>
-      </c>
-      <c r="D31" s="13">
-        <v>474503863.66666698</v>
-      </c>
-      <c r="E31" s="5">
-        <f>C31/$E$27/$E$27</f>
-        <v>39.448796296388892</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" s="3">
+      <c r="C58" s="13">
+        <v>141956</v>
+      </c>
+      <c r="D58" s="13">
+        <v>472010640</v>
+      </c>
+      <c r="E58" s="5">
+        <f>C58/$E$36/$E$36</f>
+        <v>39.432222222222222</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" s="3">
         <v>0.05</v>
       </c>
-      <c r="C32" s="13">
-        <v>622421</v>
-      </c>
-      <c r="D32" s="13">
-        <v>2912721758.1428499</v>
-      </c>
-      <c r="E32" s="5">
-        <f>C32/$E$27/$E$27</f>
-        <v>172.89472222222221</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B33" s="6">
+      <c r="C59" s="13">
+        <v>622980</v>
+      </c>
+      <c r="D59" s="13">
+        <v>2960532000</v>
+      </c>
+      <c r="E59" s="5">
+        <f>C59/$E$36/$E$36</f>
+        <v>173.05</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B60" s="6">
         <v>0.1</v>
       </c>
-      <c r="C33" s="14">
-        <v>1249198.733333</v>
-      </c>
-      <c r="D33" s="14">
-        <v>2165148774.0666599</v>
-      </c>
-      <c r="E33" s="8">
-        <f>C33/$E$27/$E$27</f>
-        <v>346.99964814805554</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9">
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B36" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9">
-      <c r="B37" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C37" s="13">
-        <v>8520940</v>
-      </c>
-      <c r="D37" s="13">
-        <v>1708213909200</v>
-      </c>
-      <c r="E37" s="5">
-        <f>C37/$E$27/$E$27</f>
-        <v>2366.9277777777775</v>
-      </c>
-      <c r="I37" s="22"/>
-    </row>
-    <row r="38" spans="2:9">
-      <c r="B38" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="C38" s="13">
-        <v>37345260</v>
-      </c>
-      <c r="D38" s="13">
-        <v>10485798329314.199</v>
-      </c>
-      <c r="E38" s="5">
-        <f>C38/$E$27/$E$27</f>
-        <v>10373.683333333332</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B39" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C39" s="14">
-        <v>74951924</v>
-      </c>
-      <c r="D39" s="14">
-        <v>7794535586640</v>
-      </c>
-      <c r="E39" s="8">
-        <f>C39/$E$27/$E$27</f>
-        <v>20819.978888888891</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B42" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9">
-      <c r="B43" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C43" s="13">
-        <v>2365.9333329999999</v>
-      </c>
-      <c r="D43" s="13">
-        <v>131114.06666700001</v>
-      </c>
-      <c r="E43" s="5">
-        <f>C43/$E$27/$E$27</f>
-        <v>0.65720370361111113</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="C44" s="13">
-        <v>10383</v>
-      </c>
-      <c r="D44" s="13">
-        <v>822370</v>
-      </c>
-      <c r="E44" s="5">
-        <f>C44/$E$27/$E$27</f>
-        <v>2.8841666666666668</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B45" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C45" s="14">
-        <v>20835.866666999998</v>
-      </c>
-      <c r="D45" s="14">
-        <v>7794535586640</v>
-      </c>
-      <c r="E45" s="8">
-        <f>C45/$E$27/$E$27</f>
-        <v>5.7877407408333328</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9">
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B48" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C49" s="13">
-        <v>141956</v>
-      </c>
-      <c r="D49" s="13">
-        <v>472010640</v>
-      </c>
-      <c r="E49" s="5">
-        <f>C49/$E$27/$E$27</f>
-        <v>39.432222222222222</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="C50" s="13">
-        <v>622980</v>
-      </c>
-      <c r="D50" s="13">
-        <v>2960532000</v>
-      </c>
-      <c r="E50" s="5">
-        <f>C50/$E$27/$E$27</f>
-        <v>173.05</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B51" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C51" s="14">
+      <c r="C60" s="14">
         <v>1250152</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D60" s="14">
         <v>2135479817.1428499</v>
       </c>
-      <c r="E51" s="8">
-        <f>C51/$E$27/$E$27</f>
+      <c r="E60" s="8">
+        <f>C60/$E$36/$E$36</f>
         <v>347.26444444444439</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2760,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D67"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
corrected AccessCount for slow MatrixPot
</commit_message>
<xml_diff>
--- a/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
+++ b/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>AccessCount</t>
   </si>
@@ -160,183 +160,6 @@
   </si>
   <si>
     <t>AccessCount - Alternativ</t>
-  </si>
-  <si>
-    <t>1852.0</t>
-  </si>
-  <si>
-    <t>112972.0</t>
-  </si>
-  <si>
-    <t>224092.0</t>
-  </si>
-  <si>
-    <t>335212.0</t>
-  </si>
-  <si>
-    <t>446332.0</t>
-  </si>
-  <si>
-    <t>557452.0</t>
-  </si>
-  <si>
-    <t>668572.0</t>
-  </si>
-  <si>
-    <t>779692.0</t>
-  </si>
-  <si>
-    <t>890812.0</t>
-  </si>
-  <si>
-    <t>1001932.0</t>
-  </si>
-  <si>
-    <t>1113052.0</t>
-  </si>
-  <si>
-    <t>1224172.0</t>
-  </si>
-  <si>
-    <t>1335292.0</t>
-  </si>
-  <si>
-    <t>1446412.0</t>
-  </si>
-  <si>
-    <t>1557532.0</t>
-  </si>
-  <si>
-    <t>1668652.0</t>
-  </si>
-  <si>
-    <t>1779772.0</t>
-  </si>
-  <si>
-    <t>1890892.0</t>
-  </si>
-  <si>
-    <t>2002012.0</t>
-  </si>
-  <si>
-    <t>2113132.0</t>
-  </si>
-  <si>
-    <t>2224252.0</t>
-  </si>
-  <si>
-    <t>2335372.0</t>
-  </si>
-  <si>
-    <t>2446492.0</t>
-  </si>
-  <si>
-    <t>2557612.0</t>
-  </si>
-  <si>
-    <t>2668732.0</t>
-  </si>
-  <si>
-    <t>2779852.0</t>
-  </si>
-  <si>
-    <t>2890972.0</t>
-  </si>
-  <si>
-    <t>3002092.0</t>
-  </si>
-  <si>
-    <t>3113212.0</t>
-  </si>
-  <si>
-    <t>3224332.0</t>
-  </si>
-  <si>
-    <t>3335452.0</t>
-  </si>
-  <si>
-    <t>3446572.0</t>
-  </si>
-  <si>
-    <t>3557692.0</t>
-  </si>
-  <si>
-    <t>3668812.0</t>
-  </si>
-  <si>
-    <t>3779932.0</t>
-  </si>
-  <si>
-    <t>3891052.0</t>
-  </si>
-  <si>
-    <t>4002172.0</t>
-  </si>
-  <si>
-    <t>4113292.0</t>
-  </si>
-  <si>
-    <t>4224412.0</t>
-  </si>
-  <si>
-    <t>4335532.0</t>
-  </si>
-  <si>
-    <t>4446652.0</t>
-  </si>
-  <si>
-    <t>4557772.0</t>
-  </si>
-  <si>
-    <t>4668892.0</t>
-  </si>
-  <si>
-    <t>4780012.0</t>
-  </si>
-  <si>
-    <t>4891132.0</t>
-  </si>
-  <si>
-    <t>5002252.0</t>
-  </si>
-  <si>
-    <t>5113372.0</t>
-  </si>
-  <si>
-    <t>5224492.0</t>
-  </si>
-  <si>
-    <t>5335612.0</t>
-  </si>
-  <si>
-    <t>5446732.0</t>
-  </si>
-  <si>
-    <t>5557852.0</t>
-  </si>
-  <si>
-    <t>5668972.0</t>
-  </si>
-  <si>
-    <t>5780092.0</t>
-  </si>
-  <si>
-    <t>5891212.0</t>
-  </si>
-  <si>
-    <t>6002332.0</t>
-  </si>
-  <si>
-    <t>6113452.0</t>
-  </si>
-  <si>
-    <t>6224572.0</t>
-  </si>
-  <si>
-    <t>6335692.0</t>
-  </si>
-  <si>
-    <t>6446812.0</t>
   </si>
   <si>
     <t>1&lt;=k&lt;=59</t>
@@ -650,25 +473,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64262912"/>
-        <c:axId val="64264448"/>
+        <c:axId val="61838080"/>
+        <c:axId val="61839616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64262912"/>
+        <c:axId val="61838080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64264448"/>
+        <c:crossAx val="61839616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64264448"/>
+        <c:axId val="61839616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +499,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64262912"/>
+        <c:crossAx val="61838080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -688,7 +511,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -704,10 +527,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10812550723840994"/>
+          <c:x val="0.10812550723840998"/>
           <c:y val="0.14061001832402045"/>
-          <c:w val="0.64893491042327456"/>
-          <c:h val="0.77567520489538855"/>
+          <c:w val="0.64893491042327489"/>
+          <c:h val="0.77567520489538877"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -787,25 +610,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="67087744"/>
-        <c:axId val="67105920"/>
+        <c:axId val="63090048"/>
+        <c:axId val="63108224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67087744"/>
+        <c:axId val="63090048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67105920"/>
+        <c:crossAx val="63108224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67105920"/>
+        <c:axId val="63108224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,20 +636,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67087744"/>
+        <c:crossAx val="63090048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -971,25 +793,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="68184704"/>
-        <c:axId val="68194688"/>
+        <c:axId val="66022016"/>
+        <c:axId val="66032000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68184704"/>
+        <c:axId val="66022016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68194688"/>
+        <c:crossAx val="66032000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68194688"/>
+        <c:axId val="66032000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -998,7 +820,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68184704"/>
+        <c:crossAx val="66022016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1010,7 +832,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1137,25 +959,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="68220800"/>
-        <c:axId val="68222336"/>
+        <c:axId val="67372928"/>
+        <c:axId val="67374464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68220800"/>
+        <c:axId val="67372928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68222336"/>
+        <c:crossAx val="67374464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68222336"/>
+        <c:axId val="67374464"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1164,7 +986,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68220800"/>
+        <c:crossAx val="67372928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1176,7 +998,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1778,25 +1600,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78249984"/>
-        <c:axId val="78251520"/>
+        <c:axId val="67432448"/>
+        <c:axId val="67433984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78249984"/>
+        <c:axId val="67432448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78251520"/>
+        <c:crossAx val="67433984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78251520"/>
+        <c:axId val="67433984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1804,20 +1626,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78249984"/>
+        <c:crossAx val="67432448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2981,8 +2802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3695,10 +3516,10 @@
     </row>
     <row r="78" spans="1:4">
       <c r="B78" s="1" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1">
@@ -3716,753 +3537,399 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="B81" s="25">
-        <v>1</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D81" s="24" t="s">
-        <v>48</v>
-      </c>
+      <c r="B81" s="25"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="24"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="B82" s="25">
-        <v>2</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D82" s="24" t="s">
-        <v>48</v>
-      </c>
+      <c r="B82" s="25"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="24"/>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="22"/>
-      <c r="B83" s="25">
-        <v>3</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D83" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B83" s="25"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="26"/>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="22"/>
-      <c r="B84" s="25">
-        <v>4</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>48</v>
-      </c>
+      <c r="B84" s="25"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="26"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="22"/>
-      <c r="B85" s="25">
-        <v>5</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D85" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B85" s="25"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="26"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="22"/>
-      <c r="B86" s="25">
-        <v>6</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D86" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B86" s="25"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="26"/>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="22"/>
-      <c r="B87" s="25">
-        <v>7</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D87" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B87" s="25"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="26"/>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="22"/>
-      <c r="B88" s="25">
-        <v>8</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D88" s="26" t="s">
-        <v>48</v>
-      </c>
+      <c r="B88" s="25"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="26"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="22"/>
-      <c r="B89" s="25">
-        <v>9</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B89" s="25"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="26"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="22"/>
-      <c r="B90" s="25">
-        <v>10</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D90" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B90" s="25"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="26"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="22"/>
-      <c r="B91" s="25">
-        <v>11</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D91" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B91" s="25"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="26"/>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="22"/>
-      <c r="B92" s="25">
-        <v>12</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D92" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B92" s="25"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="26"/>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="22"/>
-      <c r="B93" s="25">
-        <v>13</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D93" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B93" s="25"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="26"/>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="22"/>
-      <c r="B94" s="25">
-        <v>14</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D94" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B94" s="25"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="26"/>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="22"/>
-      <c r="B95" s="25">
-        <v>15</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D95" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B95" s="25"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="26"/>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="22"/>
-      <c r="B96" s="25">
-        <v>16</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D96" s="26" t="s">
-        <v>48</v>
-      </c>
+      <c r="B96" s="25"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="26"/>
       <c r="E96" s="22"/>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="22"/>
-      <c r="B97" s="25">
-        <v>17</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D97" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B97" s="25"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="26"/>
       <c r="E97" s="22"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="22"/>
-      <c r="B98" s="25">
-        <v>18</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D98" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B98" s="25"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="26"/>
       <c r="E98" s="22"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="22"/>
-      <c r="B99" s="25">
-        <v>19</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D99" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B99" s="25"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="26"/>
       <c r="E99" s="22"/>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="22"/>
-      <c r="B100" s="25">
-        <v>20</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D100" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B100" s="25"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="26"/>
       <c r="E100" s="22"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="22"/>
-      <c r="B101" s="25">
-        <v>21</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D101" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B101" s="25"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="26"/>
       <c r="E101" s="22"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="22"/>
-      <c r="B102" s="25">
-        <v>22</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D102" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B102" s="25"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="26"/>
       <c r="E102" s="22"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="22"/>
-      <c r="B103" s="25">
-        <v>23</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D103" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B103" s="25"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="26"/>
       <c r="E103" s="22"/>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="22"/>
-      <c r="B104" s="25">
-        <v>24</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D104" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B104" s="25"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="26"/>
       <c r="E104" s="22"/>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="22"/>
-      <c r="B105" s="25">
-        <v>25</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D105" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B105" s="25"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="26"/>
       <c r="E105" s="22"/>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="22"/>
-      <c r="B106" s="25">
-        <v>26</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D106" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B106" s="25"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="26"/>
       <c r="E106" s="22"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="22"/>
-      <c r="B107" s="25">
-        <v>27</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D107" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B107" s="25"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="26"/>
       <c r="E107" s="22"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="22"/>
-      <c r="B108" s="25">
-        <v>28</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D108" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B108" s="25"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="26"/>
       <c r="E108" s="22"/>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="22"/>
-      <c r="B109" s="25">
-        <v>29</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D109" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B109" s="25"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="26"/>
       <c r="E109" s="22"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="22"/>
-      <c r="B110" s="25">
-        <v>30</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D110" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B110" s="25"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="26"/>
       <c r="E110" s="22"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="22"/>
-      <c r="B111" s="25">
-        <v>31</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D111" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="B111" s="25"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="26"/>
       <c r="E111" s="22"/>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="22"/>
-      <c r="B112" s="25">
-        <v>32</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D112" s="26" t="s">
-        <v>48</v>
-      </c>
+      <c r="B112" s="25"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="26"/>
       <c r="E112" s="22"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="22"/>
-      <c r="B113" s="25">
-        <v>33</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D113" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B113" s="25"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="26"/>
       <c r="E113" s="22"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="22"/>
-      <c r="B114" s="25">
-        <v>34</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D114" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B114" s="25"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="26"/>
       <c r="E114" s="22"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="22"/>
-      <c r="B115" s="25">
-        <v>35</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D115" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B115" s="25"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="26"/>
       <c r="E115" s="22"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="22"/>
-      <c r="B116" s="25">
-        <v>36</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D116" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B116" s="25"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="26"/>
       <c r="E116" s="22"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="22"/>
-      <c r="B117" s="25">
-        <v>37</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D117" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B117" s="25"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="26"/>
       <c r="E117" s="22"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="22"/>
-      <c r="B118" s="25">
-        <v>38</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D118" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B118" s="25"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="26"/>
       <c r="E118" s="22"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="22"/>
-      <c r="B119" s="25">
-        <v>39</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D119" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B119" s="25"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="26"/>
       <c r="E119" s="22"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="22"/>
-      <c r="B120" s="25">
-        <v>40</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D120" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B120" s="25"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="26"/>
       <c r="E120" s="22"/>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="22"/>
-      <c r="B121" s="25">
-        <v>41</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D121" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B121" s="25"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="26"/>
       <c r="E121" s="22"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="22"/>
-      <c r="B122" s="25">
-        <v>42</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D122" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B122" s="25"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="26"/>
       <c r="E122" s="22"/>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="22"/>
-      <c r="B123" s="25">
-        <v>43</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D123" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B123" s="25"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="26"/>
       <c r="E123" s="22"/>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="22"/>
-      <c r="B124" s="25">
-        <v>44</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D124" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B124" s="25"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="26"/>
       <c r="E124" s="22"/>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="22"/>
-      <c r="B125" s="25">
-        <v>45</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D125" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B125" s="25"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="26"/>
       <c r="E125" s="22"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="22"/>
-      <c r="B126" s="25">
-        <v>46</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D126" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B126" s="25"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="26"/>
       <c r="E126" s="22"/>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="22"/>
-      <c r="B127" s="25">
-        <v>47</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D127" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="B127" s="25"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="26"/>
       <c r="E127" s="22"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="22"/>
-      <c r="B128" s="25">
-        <v>48</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D128" s="26" t="s">
-        <v>49</v>
-      </c>
+      <c r="B128" s="25"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="26"/>
       <c r="E128" s="22"/>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="22"/>
-      <c r="B129" s="25">
-        <v>49</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D129" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B129" s="25"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="26"/>
       <c r="E129" s="22"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="22"/>
-      <c r="B130" s="25">
-        <v>50</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D130" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B130" s="25"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="26"/>
       <c r="E130" s="22"/>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="22"/>
-      <c r="B131" s="25">
-        <v>51</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D131" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B131" s="25"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="26"/>
       <c r="E131" s="22"/>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="22"/>
-      <c r="B132" s="25">
-        <v>52</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D132" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B132" s="25"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="26"/>
       <c r="E132" s="22"/>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="22"/>
-      <c r="B133" s="25">
-        <v>53</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D133" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B133" s="25"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="26"/>
       <c r="E133" s="22"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="22"/>
-      <c r="B134" s="25">
-        <v>54</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D134" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B134" s="25"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="26"/>
       <c r="E134" s="22"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="22"/>
-      <c r="B135" s="25">
-        <v>55</v>
-      </c>
-      <c r="C135" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D135" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="B135" s="25"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="26"/>
       <c r="E135" s="22"/>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="22"/>
-      <c r="B136" s="25">
-        <v>56</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D136" s="26" t="s">
-        <v>50</v>
-      </c>
+      <c r="B136" s="25"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="26"/>
       <c r="E136" s="22"/>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="22"/>
-      <c r="B137" s="25">
-        <v>57</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D137" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B137" s="25"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="26"/>
       <c r="E137" s="22"/>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="22"/>
-      <c r="B138" s="25">
-        <v>58</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D138" s="26" t="s">
-        <v>51</v>
-      </c>
+      <c r="B138" s="25"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="26"/>
       <c r="E138" s="22"/>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="22"/>
-      <c r="B139" s="25">
-        <v>59</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D139" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="B139" s="25"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="26"/>
       <c r="E139" s="22"/>
     </row>
     <row r="140" spans="1:5">

</xml_diff>

<commit_message>
Aufgabe 4 exp- finished. TODO: write text for it
</commit_message>
<xml_diff>
--- a/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
+++ b/AD/SwaneetMatthias/AD-Excel-Sheets.xlsx
@@ -162,10 +162,10 @@
     <t>AccessCount - Alternativ</t>
   </si>
   <si>
-    <t>1&lt;=k&lt;=59</t>
+    <t>n = 45</t>
   </si>
   <si>
-    <t>n = 60</t>
+    <t>1&lt;=k&lt;n</t>
   </si>
 </sst>
 </file>
@@ -363,9 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,6 +373,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -473,25 +473,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="61838080"/>
-        <c:axId val="61839616"/>
+        <c:axId val="71209728"/>
+        <c:axId val="71211264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61838080"/>
+        <c:axId val="71209728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61839616"/>
+        <c:crossAx val="71211264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61839616"/>
+        <c:axId val="71211264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +499,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61838080"/>
+        <c:crossAx val="71209728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -511,7 +511,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -527,10 +527,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10812550723840998"/>
+          <c:x val="0.10812550723841002"/>
           <c:y val="0.14061001832402045"/>
-          <c:w val="0.64893491042327489"/>
-          <c:h val="0.77567520489538877"/>
+          <c:w val="0.64893491042327511"/>
+          <c:h val="0.77567520489538899"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -610,25 +610,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63090048"/>
-        <c:axId val="63108224"/>
+        <c:axId val="71802240"/>
+        <c:axId val="71824512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63090048"/>
+        <c:axId val="71802240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63108224"/>
+        <c:crossAx val="71824512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63108224"/>
+        <c:axId val="71824512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +636,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63090048"/>
+        <c:crossAx val="71802240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -648,7 +648,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -793,25 +793,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66022016"/>
-        <c:axId val="66032000"/>
+        <c:axId val="74930816"/>
+        <c:axId val="74940800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66022016"/>
+        <c:axId val="74930816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66032000"/>
+        <c:crossAx val="74940800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66032000"/>
+        <c:axId val="74940800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -820,7 +820,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66022016"/>
+        <c:crossAx val="74930816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -832,7 +832,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -959,25 +959,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="67372928"/>
-        <c:axId val="67374464"/>
+        <c:axId val="74971008"/>
+        <c:axId val="74972544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67372928"/>
+        <c:axId val="74971008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67374464"/>
+        <c:crossAx val="74972544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67374464"/>
+        <c:axId val="74972544"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -986,7 +986,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67372928"/>
+        <c:crossAx val="74971008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -998,7 +998,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1600,25 +1600,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="67432448"/>
-        <c:axId val="67433984"/>
+        <c:axId val="48427008"/>
+        <c:axId val="48428544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67432448"/>
+        <c:axId val="48427008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67433984"/>
+        <c:crossAx val="48428544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67433984"/>
+        <c:axId val="48428544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,19 +1626,658 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67432448"/>
+        <c:crossAx val="48427008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>AccessCount - Normal</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Aufgb3!$B$81:$B$124</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Aufgb3!$C$81:$C$124</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>874</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77590</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>133952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>182296</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226588</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>270880</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>315172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>359464</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>403756</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>448048</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>492340</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>536632</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>580924</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>625216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>669508</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>713800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>758092</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>802384</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>846676</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>890968</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>935260</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>979552</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1023844</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1068136</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1112428</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1156720</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1201012</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1245304</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1289596</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1333888</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1378180</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1422472</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1466764</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1511056</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1555348</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1599640</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1643932</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1688224</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1732516</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1776808</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1821100</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1865392</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1909684</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1953976</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>AccessCount Alternativ</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Aufgb3!$B$81:$B$124</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Aufgb3!$D$81:$D$124</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>874</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>267014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>311300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>307336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>351622</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>355608</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>399894</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>399894</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>444180</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>395930</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>440216</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>440216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>484502</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>444202</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>488488</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>488488</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>532774</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>488488</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>532774</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>532774</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>577060</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>484524</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>528810</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>528810</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>573096</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>528810</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>573096</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>573096</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>617382</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>532796</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>577082</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>577082</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>621368</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>577082</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>621368</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>621368</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>665654</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>577082</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>621368</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>621368</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>665654</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>621368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="79497472"/>
+        <c:axId val="79555584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79497472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79555584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79555584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79497472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1801,6 +2440,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>503465</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>176894</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2802,8 +3471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="C80" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3516,10 +4185,10 @@
     </row>
     <row r="78" spans="1:4">
       <c r="B78" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1">
@@ -3537,427 +4206,691 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="B81" s="25"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="24"/>
+      <c r="B81" s="26">
+        <v>1</v>
+      </c>
+      <c r="C81" s="27">
+        <v>874</v>
+      </c>
+      <c r="D81" s="28">
+        <v>874</v>
+      </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="B82" s="25"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="24"/>
+      <c r="B82" s="26">
+        <v>2</v>
+      </c>
+      <c r="C82" s="27">
+        <v>77590</v>
+      </c>
+      <c r="D82" s="28">
+        <v>154292</v>
+      </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="22"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="26"/>
+      <c r="B83" s="26">
+        <v>3</v>
+      </c>
+      <c r="C83" s="27">
+        <v>133952</v>
+      </c>
+      <c r="D83" s="27">
+        <v>210640</v>
+      </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="22"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="26"/>
+      <c r="B84" s="26">
+        <v>4</v>
+      </c>
+      <c r="C84" s="27">
+        <v>182296</v>
+      </c>
+      <c r="D84" s="27">
+        <v>267014</v>
+      </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="22"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="26"/>
+      <c r="B85" s="26">
+        <v>5</v>
+      </c>
+      <c r="C85" s="27">
+        <v>226588</v>
+      </c>
+      <c r="D85" s="27">
+        <v>311300</v>
+      </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="22"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="26"/>
+      <c r="B86" s="26">
+        <v>6</v>
+      </c>
+      <c r="C86" s="27">
+        <v>270880</v>
+      </c>
+      <c r="D86" s="27">
+        <v>307336</v>
+      </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="22"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="26"/>
+      <c r="B87" s="26">
+        <v>7</v>
+      </c>
+      <c r="C87" s="27">
+        <v>315172</v>
+      </c>
+      <c r="D87" s="27">
+        <v>351622</v>
+      </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="22"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="26"/>
+      <c r="B88" s="26">
+        <v>8</v>
+      </c>
+      <c r="C88" s="27">
+        <v>359464</v>
+      </c>
+      <c r="D88" s="27">
+        <v>355608</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="22"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="26"/>
+      <c r="B89" s="26">
+        <v>9</v>
+      </c>
+      <c r="C89" s="27">
+        <v>403756</v>
+      </c>
+      <c r="D89" s="27">
+        <v>399894</v>
+      </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="22"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="26"/>
+      <c r="B90" s="26">
+        <v>10</v>
+      </c>
+      <c r="C90" s="27">
+        <v>448048</v>
+      </c>
+      <c r="D90" s="27">
+        <v>399894</v>
+      </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="22"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="26"/>
+      <c r="B91" s="26">
+        <v>11</v>
+      </c>
+      <c r="C91" s="27">
+        <v>492340</v>
+      </c>
+      <c r="D91" s="27">
+        <v>444180</v>
+      </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="22"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="26"/>
+      <c r="B92" s="26">
+        <v>12</v>
+      </c>
+      <c r="C92" s="27">
+        <v>536632</v>
+      </c>
+      <c r="D92" s="27">
+        <v>395930</v>
+      </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="22"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="26"/>
+      <c r="B93" s="26">
+        <v>13</v>
+      </c>
+      <c r="C93" s="27">
+        <v>580924</v>
+      </c>
+      <c r="D93" s="27">
+        <v>440216</v>
+      </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="22"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="26"/>
+      <c r="B94" s="26">
+        <v>14</v>
+      </c>
+      <c r="C94" s="27">
+        <v>625216</v>
+      </c>
+      <c r="D94" s="27">
+        <v>440216</v>
+      </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="22"/>
-      <c r="B95" s="25"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="26"/>
+      <c r="B95" s="26">
+        <v>15</v>
+      </c>
+      <c r="C95" s="27">
+        <v>669508</v>
+      </c>
+      <c r="D95" s="27">
+        <v>484502</v>
+      </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="22"/>
-      <c r="B96" s="25"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="26"/>
+      <c r="B96" s="26">
+        <v>16</v>
+      </c>
+      <c r="C96" s="27">
+        <v>713800</v>
+      </c>
+      <c r="D96" s="27">
+        <v>444202</v>
+      </c>
       <c r="E96" s="22"/>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="22"/>
-      <c r="B97" s="25"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="26"/>
+      <c r="B97" s="26">
+        <v>17</v>
+      </c>
+      <c r="C97" s="27">
+        <v>758092</v>
+      </c>
+      <c r="D97" s="27">
+        <v>488488</v>
+      </c>
       <c r="E97" s="22"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="22"/>
-      <c r="B98" s="25"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="26"/>
+      <c r="B98" s="26">
+        <v>18</v>
+      </c>
+      <c r="C98" s="27">
+        <v>802384</v>
+      </c>
+      <c r="D98" s="27">
+        <v>488488</v>
+      </c>
       <c r="E98" s="22"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="22"/>
-      <c r="B99" s="25"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="26"/>
+      <c r="B99" s="26">
+        <v>19</v>
+      </c>
+      <c r="C99" s="27">
+        <v>846676</v>
+      </c>
+      <c r="D99" s="27">
+        <v>532774</v>
+      </c>
       <c r="E99" s="22"/>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="22"/>
-      <c r="B100" s="25"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="26"/>
+      <c r="B100" s="26">
+        <v>20</v>
+      </c>
+      <c r="C100" s="27">
+        <v>890968</v>
+      </c>
+      <c r="D100" s="27">
+        <v>488488</v>
+      </c>
       <c r="E100" s="22"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="22"/>
-      <c r="B101" s="25"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="26"/>
+      <c r="B101" s="26">
+        <v>21</v>
+      </c>
+      <c r="C101" s="27">
+        <v>935260</v>
+      </c>
+      <c r="D101" s="27">
+        <v>532774</v>
+      </c>
       <c r="E101" s="22"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="22"/>
-      <c r="B102" s="25"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="26"/>
+      <c r="B102" s="26">
+        <v>22</v>
+      </c>
+      <c r="C102" s="27">
+        <v>979552</v>
+      </c>
+      <c r="D102" s="27">
+        <v>532774</v>
+      </c>
       <c r="E102" s="22"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="22"/>
-      <c r="B103" s="25"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="26"/>
+      <c r="B103" s="26">
+        <v>23</v>
+      </c>
+      <c r="C103" s="27">
+        <v>1023844</v>
+      </c>
+      <c r="D103" s="27">
+        <v>577060</v>
+      </c>
       <c r="E103" s="22"/>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="22"/>
-      <c r="B104" s="25"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="26"/>
+      <c r="B104" s="26">
+        <v>24</v>
+      </c>
+      <c r="C104" s="27">
+        <v>1068136</v>
+      </c>
+      <c r="D104" s="27">
+        <v>484524</v>
+      </c>
       <c r="E104" s="22"/>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="22"/>
-      <c r="B105" s="25"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="26"/>
+      <c r="B105" s="26">
+        <v>25</v>
+      </c>
+      <c r="C105" s="27">
+        <v>1112428</v>
+      </c>
+      <c r="D105" s="27">
+        <v>528810</v>
+      </c>
       <c r="E105" s="22"/>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="22"/>
-      <c r="B106" s="25"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="26"/>
+      <c r="B106" s="26">
+        <v>26</v>
+      </c>
+      <c r="C106" s="27">
+        <v>1156720</v>
+      </c>
+      <c r="D106" s="27">
+        <v>528810</v>
+      </c>
       <c r="E106" s="22"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="22"/>
-      <c r="B107" s="25"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="26"/>
+      <c r="B107" s="26">
+        <v>27</v>
+      </c>
+      <c r="C107" s="27">
+        <v>1201012</v>
+      </c>
+      <c r="D107" s="27">
+        <v>573096</v>
+      </c>
       <c r="E107" s="22"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="22"/>
-      <c r="B108" s="25"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="26"/>
+      <c r="B108" s="26">
+        <v>28</v>
+      </c>
+      <c r="C108" s="27">
+        <v>1245304</v>
+      </c>
+      <c r="D108" s="27">
+        <v>528810</v>
+      </c>
       <c r="E108" s="22"/>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="22"/>
-      <c r="B109" s="25"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="26"/>
+      <c r="B109" s="26">
+        <v>29</v>
+      </c>
+      <c r="C109" s="27">
+        <v>1289596</v>
+      </c>
+      <c r="D109" s="27">
+        <v>573096</v>
+      </c>
       <c r="E109" s="22"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="22"/>
-      <c r="B110" s="25"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="26"/>
+      <c r="B110" s="26">
+        <v>30</v>
+      </c>
+      <c r="C110" s="27">
+        <v>1333888</v>
+      </c>
+      <c r="D110" s="27">
+        <v>573096</v>
+      </c>
       <c r="E110" s="22"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="22"/>
-      <c r="B111" s="25"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="26"/>
+      <c r="B111" s="26">
+        <v>31</v>
+      </c>
+      <c r="C111" s="27">
+        <v>1378180</v>
+      </c>
+      <c r="D111" s="27">
+        <v>617382</v>
+      </c>
       <c r="E111" s="22"/>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="22"/>
-      <c r="B112" s="25"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="26"/>
+      <c r="B112" s="26">
+        <v>32</v>
+      </c>
+      <c r="C112" s="27">
+        <v>1422472</v>
+      </c>
+      <c r="D112" s="27">
+        <v>532796</v>
+      </c>
       <c r="E112" s="22"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="22"/>
-      <c r="B113" s="25"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="26"/>
+      <c r="B113" s="26">
+        <v>33</v>
+      </c>
+      <c r="C113" s="27">
+        <v>1466764</v>
+      </c>
+      <c r="D113" s="27">
+        <v>577082</v>
+      </c>
       <c r="E113" s="22"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="22"/>
-      <c r="B114" s="25"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="26"/>
+      <c r="B114" s="26">
+        <v>34</v>
+      </c>
+      <c r="C114" s="27">
+        <v>1511056</v>
+      </c>
+      <c r="D114" s="27">
+        <v>577082</v>
+      </c>
       <c r="E114" s="22"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="22"/>
-      <c r="B115" s="25"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="26"/>
+      <c r="B115" s="26">
+        <v>35</v>
+      </c>
+      <c r="C115" s="27">
+        <v>1555348</v>
+      </c>
+      <c r="D115" s="27">
+        <v>621368</v>
+      </c>
       <c r="E115" s="22"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="22"/>
-      <c r="B116" s="25"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="26"/>
+      <c r="B116" s="26">
+        <v>36</v>
+      </c>
+      <c r="C116" s="27">
+        <v>1599640</v>
+      </c>
+      <c r="D116" s="27">
+        <v>577082</v>
+      </c>
       <c r="E116" s="22"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="22"/>
-      <c r="B117" s="25"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="26"/>
+      <c r="B117" s="26">
+        <v>37</v>
+      </c>
+      <c r="C117" s="27">
+        <v>1643932</v>
+      </c>
+      <c r="D117" s="27">
+        <v>621368</v>
+      </c>
       <c r="E117" s="22"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="22"/>
-      <c r="B118" s="25"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="26"/>
+      <c r="B118" s="26">
+        <v>38</v>
+      </c>
+      <c r="C118" s="27">
+        <v>1688224</v>
+      </c>
+      <c r="D118" s="27">
+        <v>621368</v>
+      </c>
       <c r="E118" s="22"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="22"/>
-      <c r="B119" s="25"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="26"/>
+      <c r="B119" s="26">
+        <v>39</v>
+      </c>
+      <c r="C119" s="27">
+        <v>1732516</v>
+      </c>
+      <c r="D119" s="27">
+        <v>665654</v>
+      </c>
       <c r="E119" s="22"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="22"/>
-      <c r="B120" s="25"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="26"/>
+      <c r="B120" s="26">
+        <v>40</v>
+      </c>
+      <c r="C120" s="27">
+        <v>1776808</v>
+      </c>
+      <c r="D120" s="27">
+        <v>577082</v>
+      </c>
       <c r="E120" s="22"/>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="22"/>
-      <c r="B121" s="25"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="26"/>
+      <c r="B121" s="26">
+        <v>41</v>
+      </c>
+      <c r="C121" s="27">
+        <v>1821100</v>
+      </c>
+      <c r="D121" s="27">
+        <v>621368</v>
+      </c>
       <c r="E121" s="22"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="22"/>
-      <c r="B122" s="25"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="26"/>
+      <c r="B122" s="26">
+        <v>42</v>
+      </c>
+      <c r="C122" s="27">
+        <v>1865392</v>
+      </c>
+      <c r="D122" s="27">
+        <v>621368</v>
+      </c>
       <c r="E122" s="22"/>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="22"/>
-      <c r="B123" s="25"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="26"/>
+      <c r="B123" s="26">
+        <v>43</v>
+      </c>
+      <c r="C123" s="27">
+        <v>1909684</v>
+      </c>
+      <c r="D123" s="27">
+        <v>665654</v>
+      </c>
       <c r="E123" s="22"/>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="22"/>
-      <c r="B124" s="25"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="26"/>
+      <c r="B124" s="26">
+        <v>44</v>
+      </c>
+      <c r="C124" s="27">
+        <v>1953976</v>
+      </c>
+      <c r="D124" s="27">
+        <v>621368</v>
+      </c>
       <c r="E124" s="22"/>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="22"/>
-      <c r="B125" s="25"/>
+      <c r="B125" s="24"/>
       <c r="C125" s="4"/>
-      <c r="D125" s="26"/>
+      <c r="D125" s="25"/>
       <c r="E125" s="22"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="22"/>
-      <c r="B126" s="25"/>
+      <c r="B126" s="24"/>
       <c r="C126" s="4"/>
-      <c r="D126" s="26"/>
+      <c r="D126" s="25"/>
       <c r="E126" s="22"/>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="22"/>
-      <c r="B127" s="25"/>
+      <c r="B127" s="24"/>
       <c r="C127" s="4"/>
-      <c r="D127" s="26"/>
+      <c r="D127" s="25"/>
       <c r="E127" s="22"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="22"/>
-      <c r="B128" s="25"/>
+      <c r="B128" s="24"/>
       <c r="C128" s="4"/>
-      <c r="D128" s="26"/>
+      <c r="D128" s="25"/>
       <c r="E128" s="22"/>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="22"/>
-      <c r="B129" s="25"/>
+      <c r="B129" s="24"/>
       <c r="C129" s="4"/>
-      <c r="D129" s="26"/>
+      <c r="D129" s="25"/>
       <c r="E129" s="22"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="22"/>
-      <c r="B130" s="25"/>
+      <c r="B130" s="24"/>
       <c r="C130" s="4"/>
-      <c r="D130" s="26"/>
+      <c r="D130" s="25"/>
       <c r="E130" s="22"/>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="22"/>
-      <c r="B131" s="25"/>
+      <c r="B131" s="24"/>
       <c r="C131" s="4"/>
-      <c r="D131" s="26"/>
+      <c r="D131" s="25"/>
       <c r="E131" s="22"/>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="22"/>
-      <c r="B132" s="25"/>
+      <c r="B132" s="24"/>
       <c r="C132" s="4"/>
-      <c r="D132" s="26"/>
+      <c r="D132" s="25"/>
       <c r="E132" s="22"/>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="22"/>
-      <c r="B133" s="25"/>
+      <c r="B133" s="24"/>
       <c r="C133" s="4"/>
-      <c r="D133" s="26"/>
+      <c r="D133" s="25"/>
       <c r="E133" s="22"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="22"/>
-      <c r="B134" s="25"/>
+      <c r="B134" s="24"/>
       <c r="C134" s="4"/>
-      <c r="D134" s="26"/>
+      <c r="D134" s="25"/>
       <c r="E134" s="22"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="22"/>
-      <c r="B135" s="25"/>
+      <c r="B135" s="24"/>
       <c r="C135" s="4"/>
-      <c r="D135" s="26"/>
+      <c r="D135" s="25"/>
       <c r="E135" s="22"/>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="22"/>
-      <c r="B136" s="25"/>
+      <c r="B136" s="24"/>
       <c r="C136" s="4"/>
-      <c r="D136" s="26"/>
+      <c r="D136" s="25"/>
       <c r="E136" s="22"/>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="22"/>
-      <c r="B137" s="25"/>
+      <c r="B137" s="24"/>
       <c r="C137" s="4"/>
-      <c r="D137" s="26"/>
+      <c r="D137" s="25"/>
       <c r="E137" s="22"/>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="22"/>
-      <c r="B138" s="25"/>
+      <c r="B138" s="24"/>
       <c r="C138" s="4"/>
-      <c r="D138" s="26"/>
+      <c r="D138" s="25"/>
       <c r="E138" s="22"/>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="22"/>
-      <c r="B139" s="25"/>
+      <c r="B139" s="24"/>
       <c r="C139" s="4"/>
-      <c r="D139" s="26"/>
+      <c r="D139" s="25"/>
       <c r="E139" s="22"/>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="22"/>
-      <c r="B140" s="27"/>
+      <c r="B140" s="26"/>
       <c r="C140" s="22"/>
       <c r="D140" s="22"/>
       <c r="E140" s="22"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="22"/>
-      <c r="B141" s="27"/>
+      <c r="B141" s="26"/>
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
       <c r="E141" s="22"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="22"/>
-      <c r="B142" s="27"/>
+      <c r="B142" s="26"/>
       <c r="C142" s="22"/>
       <c r="D142" s="22"/>
       <c r="E142" s="22"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="22"/>
-      <c r="B143" s="27"/>
-      <c r="C143" s="28"/>
-      <c r="D143" s="28"/>
+      <c r="B143" s="26"/>
+      <c r="C143" s="27"/>
+      <c r="D143" s="27"/>
       <c r="E143" s="22"/>
     </row>
     <row r="144" spans="1:5">
@@ -3991,8 +4924,8 @@
     <row r="148" spans="1:5">
       <c r="A148" s="22"/>
       <c r="B148" s="4"/>
-      <c r="C148" s="28"/>
-      <c r="D148" s="28"/>
+      <c r="C148" s="27"/>
+      <c r="D148" s="27"/>
       <c r="E148" s="22"/>
     </row>
     <row r="149" spans="1:5">
@@ -4026,8 +4959,8 @@
     <row r="153" spans="1:5">
       <c r="A153" s="22"/>
       <c r="B153" s="4"/>
-      <c r="C153" s="28"/>
-      <c r="D153" s="28"/>
+      <c r="C153" s="27"/>
+      <c r="D153" s="27"/>
       <c r="E153" s="22"/>
     </row>
     <row r="154" spans="1:5">
@@ -4061,8 +4994,8 @@
     <row r="158" spans="1:5">
       <c r="A158" s="22"/>
       <c r="B158" s="4"/>
-      <c r="C158" s="28"/>
-      <c r="D158" s="28"/>
+      <c r="C158" s="27"/>
+      <c r="D158" s="27"/>
       <c r="E158" s="22"/>
     </row>
     <row r="159" spans="1:5">
@@ -4096,15 +5029,15 @@
     <row r="163" spans="1:5">
       <c r="A163" s="22"/>
       <c r="B163" s="4"/>
-      <c r="C163" s="28"/>
-      <c r="D163" s="28"/>
+      <c r="C163" s="27"/>
+      <c r="D163" s="27"/>
       <c r="E163" s="22"/>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="22"/>
       <c r="B164" s="4"/>
-      <c r="C164" s="28"/>
-      <c r="D164" s="28"/>
+      <c r="C164" s="27"/>
+      <c r="D164" s="27"/>
       <c r="E164" s="22"/>
     </row>
     <row r="165" spans="1:5">
@@ -4131,8 +5064,8 @@
     <row r="168" spans="1:5">
       <c r="A168" s="22"/>
       <c r="B168" s="4"/>
-      <c r="C168" s="28"/>
-      <c r="D168" s="28"/>
+      <c r="C168" s="27"/>
+      <c r="D168" s="27"/>
       <c r="E168" s="22"/>
     </row>
     <row r="169" spans="1:5">

</xml_diff>